<commit_message>
add: New fields added.
</commit_message>
<xml_diff>
--- a/AL_Fields_Revised.xlsx
+++ b/AL_Fields_Revised.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\gisappser2\Engineering_GIS\Domiano_Robert\USIC\PythonScripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F2BA60-3B5C-44F5-AB09-1FA191AAB76F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51584A38-665F-4465-A802-DE05932904C6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{367E046B-1E4C-49F6-BAFA-71796CED2EB1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9300" uniqueCount="1726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9439" uniqueCount="1747">
   <si>
     <t>Table</t>
   </si>
@@ -5211,6 +5211,69 @@
   </si>
   <si>
     <t>gisadmin.projectdata</t>
+  </si>
+  <si>
+    <t>gaslamp</t>
+  </si>
+  <si>
+    <t>symbolrotation</t>
+  </si>
+  <si>
+    <t>street_number</t>
+  </si>
+  <si>
+    <t>street_name</t>
+  </si>
+  <si>
+    <t>street_suffix</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>meterlocation</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Is URL field wanted?</t>
+  </si>
+  <si>
+    <t>valvetext</t>
+  </si>
+  <si>
+    <t>rontsize</t>
+  </si>
+  <si>
+    <t>casingtext</t>
+  </si>
+  <si>
+    <t>fittingtext</t>
+  </si>
+  <si>
+    <t>retiredmaintext</t>
+  </si>
+  <si>
+    <t>retiredservicetext</t>
+  </si>
+  <si>
+    <t>regulatorstationtext</t>
+  </si>
+  <si>
+    <t>stopperfittingtext</t>
+  </si>
+  <si>
+    <t>stationtype</t>
+  </si>
+  <si>
+    <t>LEADDIRECTION</t>
+  </si>
+  <si>
+    <t>LOCATIONDIRECTION</t>
+  </si>
+  <si>
+    <t>Is URL wanted for Customer shp?</t>
   </si>
 </sst>
 </file>
@@ -5263,7 +5326,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -5271,17 +5334,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5420,8 +5497,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1294518F-F526-4B7B-9FA0-AAD867AF8FD9}" name="Table1" displayName="Table1" ref="A1:C136" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:C136" xr:uid="{F75189C3-0D66-4B7E-B1E3-9B62E992FBAD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1294518F-F526-4B7B-9FA0-AAD867AF8FD9}" name="Table1" displayName="Table1" ref="A1:C204" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:C204" xr:uid="{F75189C3-0D66-4B7E-B1E3-9B62E992FBAD}"/>
   <sortState ref="A2:C109">
     <sortCondition ref="A1:A109"/>
   </sortState>
@@ -39184,20 +39261,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1E5225-34EE-4EC7-BF9B-DBF232E3BF15}">
-  <dimension ref="A1:C136"/>
+  <dimension ref="A1:G204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="F123" sqref="F123"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.88671875" customWidth="1"/>
     <col min="3" max="3" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1687</v>
       </c>
@@ -39207,8 +39284,11 @@
       <c r="C1" s="3" t="s">
         <v>1694</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -39218,8 +39298,11 @@
       <c r="C2" s="3" t="s">
         <v>1695</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -39230,7 +39313,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -39241,7 +39324,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -39252,7 +39335,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -39263,7 +39346,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -39274,7 +39357,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -39285,7 +39368,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>145</v>
       </c>
@@ -39296,7 +39379,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>145</v>
       </c>
@@ -39307,7 +39390,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>145</v>
       </c>
@@ -39318,7 +39401,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>145</v>
       </c>
@@ -39329,7 +39412,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>145</v>
       </c>
@@ -39340,7 +39423,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>145</v>
       </c>
@@ -39351,7 +39434,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>436</v>
       </c>
@@ -39362,7 +39445,7 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>436</v>
       </c>
@@ -40692,6 +40775,618 @@
       <c r="C136" s="3" t="s">
         <v>1725</v>
       </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" s="6" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C137" s="3"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" s="6" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C138" s="3"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" s="6" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C139" s="3"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" s="6" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C140" s="3"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" s="6" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C141" s="3"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" s="6" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C142" s="3"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" s="6" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C143" s="3"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" s="6" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="C144" s="3"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A145" s="6" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C145" s="3"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146" s="6" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="C146" s="3"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147" s="6" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="C147" s="3"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148" s="6" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C148" s="3"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A149" s="6" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C149" s="3"/>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A150" s="6" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C150" s="3"/>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A151" s="6" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C151" s="3"/>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A152" s="6" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C152" s="3"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A153" s="6" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C153" s="3"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A154" s="6" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C154" s="3"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A155" s="6" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C155" s="3"/>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A156" s="6" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="C156" s="3"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A157" s="6" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C157" s="3"/>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A158" s="6" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="C158" s="3"/>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A159" s="6" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="C159" s="3"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A160" s="6" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C160" s="3"/>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A161" s="6" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C161" s="3"/>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162" s="6" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C162" s="3"/>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A163" s="6" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>1743</v>
+      </c>
+      <c r="C163" s="3"/>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A164" s="6" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C164" s="3"/>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A165" s="6" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C165" s="3"/>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A166" s="6" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>1744</v>
+      </c>
+      <c r="C166" s="3"/>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A167" s="3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C167" s="3"/>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A168" s="3" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C168" s="3"/>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A169" s="3" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C169" s="3"/>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A170" s="3" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C170" s="3"/>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A171" s="3" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C171" s="3"/>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A172" s="3" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C172" s="3"/>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A173" s="3" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="C173" s="3"/>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174" s="3" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C174" s="3"/>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A175" s="3" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="C175" s="3"/>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A176" s="3" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="C176" s="3"/>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A177" s="3" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C177" s="3"/>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A178" s="3" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C178" s="3"/>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A179" s="3" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C179" s="3"/>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A180" s="3" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>1736</v>
+      </c>
+      <c r="C180" s="3"/>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A181" s="3" t="s">
+        <v>1737</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C181" s="3"/>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A182" s="3" t="s">
+        <v>1737</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C182" s="3"/>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A183" s="3" t="s">
+        <v>1737</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C183" s="3"/>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A184" s="3" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C184" s="3"/>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A185" s="3" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C185" s="3"/>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A186" s="3" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C186" s="3"/>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A187" s="3" t="s">
+        <v>1739</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C187" s="3"/>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A188" s="3" t="s">
+        <v>1739</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C188" s="3"/>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A189" s="3" t="s">
+        <v>1739</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C189" s="3"/>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A190" s="3" t="s">
+        <v>1740</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C190" s="3"/>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A191" s="3" t="s">
+        <v>1739</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C191" s="3"/>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A192" s="3" t="s">
+        <v>1739</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C192" s="3"/>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A193" s="3" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C193" s="3"/>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A194" s="3" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C194" s="3"/>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A195" s="3" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C195" s="3"/>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A196" s="3" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C196" s="3"/>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A197" s="3" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C197" s="3"/>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A198" s="3" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C198" s="3"/>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A199" s="3" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C199" s="3"/>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A200" s="3" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>1728</v>
+      </c>
+      <c r="C200" s="3"/>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A201" s="3" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>1729</v>
+      </c>
+      <c r="C201" s="3"/>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A202" s="3" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>1730</v>
+      </c>
+      <c r="C202" s="3"/>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A203" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>1732</v>
+      </c>
+      <c r="C203" s="3"/>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A204" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C204" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B101:B104">
@@ -40712,7 +41407,7 @@
           <x14:formula1>
             <xm:f>'C:\Users\09118\Desktop\[Baseline Spreadsheet AL_Fields.xlsx]Tables'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A87 A97:A98</xm:sqref>
+          <xm:sqref>A2:A87 A97:A98 A168:A177</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -40722,10 +41417,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6F9BE1-CA72-4A1E-B3E5-1D5DC86488E4}">
-  <dimension ref="A1"/>
+  <dimension ref="C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="A1:D19"/>
+      <selection activeCell="B6" sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40733,7 +41428,13 @@
     <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>1734</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update: Updates per email on 02/27 for removed fields.
</commit_message>
<xml_diff>
--- a/AL_Fields_Revised.xlsx
+++ b/AL_Fields_Revised.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\gisappser2\Engineering_GIS\Domiano_Robert\USIC\PythonScripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51584A38-665F-4465-A802-DE05932904C6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B050D2-22F9-4FD3-9F3B-060642B9CFBB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{367E046B-1E4C-49F6-BAFA-71796CED2EB1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{367E046B-1E4C-49F6-BAFA-71796CED2EB1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="6" r:id="rId1"/>
     <sheet name="RecordedFields" sheetId="4" r:id="rId2"/>
     <sheet name="FieldsToAdd" sheetId="5" r:id="rId3"/>
   </sheets>
@@ -21,7 +21,7 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$2960</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet1 (2)'!$A$1:$A$2960</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9439" uniqueCount="1747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9450" uniqueCount="1751">
   <si>
     <t>Table</t>
   </si>
@@ -5063,9 +5063,6 @@
     <t>Not send other layers?</t>
   </si>
   <si>
-    <t>Script this out.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Send layers to: \\pdatfile01\ProdData\GIS\USIC\SpireAL </t>
   </si>
   <si>
@@ -5274,6 +5271,21 @@
   </si>
   <si>
     <t>Is URL wanted for Customer shp?</t>
+  </si>
+  <si>
+    <t>Do not need. Script this out.</t>
+  </si>
+  <si>
+    <t>Related tables to stations - do not send</t>
+  </si>
+  <si>
+    <t>Use Fitting Size instead - only one is necessary for USIC</t>
+  </si>
+  <si>
+    <t>Not necessary</t>
+  </si>
+  <si>
+    <t>Not necessary - use Material Code instead</t>
   </si>
 </sst>
 </file>
@@ -5294,7 +5306,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5325,6 +5337,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -5351,19 +5369,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5381,6 +5422,14 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B050"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5421,14 +5470,6 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B050"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5497,15 +5538,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1294518F-F526-4B7B-9FA0-AAD867AF8FD9}" name="Table1" displayName="Table1" ref="A1:C204" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:C204" xr:uid="{F75189C3-0D66-4B7E-B1E3-9B62E992FBAD}"/>
-  <sortState ref="A2:C109">
-    <sortCondition ref="A1:A109"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1294518F-F526-4B7B-9FA0-AAD867AF8FD9}" name="Table1" displayName="Table1" ref="A1:C202" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:C202" xr:uid="{F75189C3-0D66-4B7E-B1E3-9B62E992FBAD}"/>
+  <sortState ref="A2:C202">
+    <sortCondition ref="A1:A202"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{B45FB957-20AF-4788-ACCE-9607C2A5885E}" name="fromTable" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{DAC79196-D75B-4C5A-BA0D-ACA19E0274C7}" name="keepList" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{A155A2E6-B443-4176-BE9B-DD01B1938F64}" name="Datalayer" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{B45FB957-20AF-4788-ACCE-9607C2A5885E}" name="fromTable" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{DAC79196-D75B-4C5A-BA0D-ACA19E0274C7}" name="keepList" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{A155A2E6-B443-4176-BE9B-DD01B1938F64}" name="Datalayer" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5807,11 +5848,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BECE847-406E-4903-805A-0359A3DCDDED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426C2F6F-D76E-4751-9350-DDCF1863B36A}">
   <dimension ref="A1:W2960"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="A24:B29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5820,7 +5862,7 @@
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="59.6640625" customWidth="1"/>
-    <col min="6" max="6" width="29.109375" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
@@ -5852,17 +5894,17 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>1676</v>
+      <c r="D3" s="6" t="s">
+        <v>1746</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
@@ -5876,7 +5918,7 @@
         <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
@@ -5921,7 +5963,7 @@
         <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -5954,7 +5996,7 @@
         <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -5989,7 +6031,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="2" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -6053,7 +6095,7 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="2" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -6086,7 +6128,7 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="2" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -6121,7 +6163,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -6295,18 +6337,19 @@
       <c r="W17" s="3"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="6" t="s">
+        <v>1747</v>
+      </c>
       <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -6326,18 +6369,19 @@
       <c r="W18" s="3"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="6" t="s">
+        <v>1747</v>
+      </c>
       <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -6357,16 +6401,18 @@
       <c r="W19" s="3"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="6" t="s">
         <v>564</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="6" t="s">
+        <v>1747</v>
+      </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -6388,16 +6434,18 @@
       <c r="W20" s="3"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="6" t="s">
         <v>564</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="6" t="s">
+        <v>1747</v>
+      </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -6636,16 +6684,18 @@
       <c r="W28" s="3"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="6" t="s">
         <v>680</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="6" t="s">
         <v>700</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="6" t="s">
         <v>700</v>
       </c>
-      <c r="D29" s="3"/>
+      <c r="D29" s="6" t="s">
+        <v>1748</v>
+      </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -6667,16 +6717,18 @@
       <c r="W29" s="3"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="6" t="s">
         <v>680</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="6" t="s">
+        <v>1749</v>
+      </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -6739,7 +6791,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>1039</v>
       </c>
@@ -6750,7 +6802,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>1039</v>
       </c>
@@ -6761,18 +6813,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
         <v>1039</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35" s="6" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>1039</v>
       </c>
@@ -6783,7 +6838,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>1039</v>
       </c>
@@ -6794,7 +6849,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>1039</v>
       </c>
@@ -6805,7 +6860,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>1039</v>
       </c>
@@ -6816,7 +6871,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>1039</v>
       </c>
@@ -6827,7 +6882,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>1039</v>
       </c>
@@ -6838,7 +6893,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>1039</v>
       </c>
@@ -6849,7 +6904,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>1039</v>
       </c>
@@ -6860,7 +6915,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>1039</v>
       </c>
@@ -6871,7 +6926,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>1039</v>
       </c>
@@ -6882,7 +6937,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>1039</v>
       </c>
@@ -6893,7 +6948,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>1234</v>
       </c>
@@ -6904,7 +6959,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>1234</v>
       </c>
@@ -7091,7 +7146,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>1339</v>
       </c>
@@ -7102,7 +7157,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>1339</v>
       </c>
@@ -7113,7 +7168,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>1339</v>
       </c>
@@ -7124,7 +7179,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>1339</v>
       </c>
@@ -7135,7 +7190,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>1339</v>
       </c>
@@ -7146,7 +7201,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>1339</v>
       </c>
@@ -7157,7 +7212,7 @@
         <v>1346</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>1339</v>
       </c>
@@ -7168,7 +7223,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>1339</v>
       </c>
@@ -7179,7 +7234,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>1373</v>
       </c>
@@ -7190,7 +7245,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>1373</v>
       </c>
@@ -7201,7 +7256,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>1373</v>
       </c>
@@ -7212,7 +7267,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>1653</v>
       </c>
@@ -7222,8 +7277,9 @@
       <c r="C76" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>1653</v>
       </c>
@@ -7234,7 +7290,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>1653</v>
       </c>
@@ -7245,7 +7301,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -7256,7 +7312,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>3</v>
       </c>
@@ -7487,7 +7543,7 @@
         <v>5</v>
       </c>
       <c r="D100" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -11725,7 +11781,7 @@
         <v>29</v>
       </c>
       <c r="D485" s="4" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="E485" s="3"/>
       <c r="F485" s="3"/>
@@ -39240,14 +39296,32 @@
   </sheetData>
   <autoFilter ref="A1:A2960" xr:uid="{23E46DE6-C876-4310-B0A6-27F6C702C110}">
     <sortState ref="A2:C2960">
-      <sortCondition sortBy="cellColor" ref="A1:A2960" dxfId="7"/>
+      <sortCondition sortBy="cellColor" ref="A1:A2960" dxfId="5"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" stopIfTrue="1" id="{A4847CDF-71AB-49E7-A273-7034878DC9FB}">
+            <xm:f>(COUNTIF(RecordedFields!B:B,B1)&gt;0)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill patternType="none">
+                  <bgColor auto="1"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>B1:B1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{9AA95E6E-EB56-4669-9725-41962562FB2F}">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{E24C35AC-A075-4B60-A662-7F995BBB8716}">
           <x14:formula1>
             <xm:f>'C:\Users\09118\Desktop\[Baseline Spreadsheet AL_Fields.xlsx]Tables'!#REF!</xm:f>
           </x14:formula1>
@@ -39261,10 +39335,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1E5225-34EE-4EC7-BF9B-DBF232E3BF15}">
-  <dimension ref="A1:G204"/>
+  <dimension ref="A1:G202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B170" sqref="B170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39276,13 +39350,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="G1" t="s">
         <v>1182</v>
@@ -39296,10 +39370,10 @@
         <v>12</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="G2" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -39307,10 +39381,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -39318,10 +39392,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -39329,10 +39403,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -39340,10 +39414,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -39351,21 +39425,21 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>3</v>
+        <v>145</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -39373,10 +39447,10 @@
         <v>145</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -39384,10 +39458,10 @@
         <v>145</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -39395,10 +39469,10 @@
         <v>145</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -39406,10 +39480,10 @@
         <v>145</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -39417,54 +39491,48 @@
         <v>145</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>156</v>
+        <v>44</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>145</v>
+        <v>1736</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>1712</v>
+      </c>
+      <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>436</v>
+        <v>1736</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>1713</v>
+      </c>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>436</v>
+        <v>1736</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>1714</v>
+      </c>
+      <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>436</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>441</v>
+        <v>10</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -39472,1928 +39540,1932 @@
         <v>436</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>44</v>
+        <v>439</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>1700</v>
+        <v>436</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>10</v>
+        <v>441</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>1700</v>
+        <v>436</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>382</v>
+        <v>44</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>1700</v>
+        <v>1730</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1690</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>1731</v>
+      </c>
+      <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>1696</v>
+        <v>1730</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1697</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>1732</v>
+      </c>
+      <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>1696</v>
+        <v>1715</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>526</v>
+        <v>10</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>1696</v>
+        <v>1715</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1698</v>
+        <v>1689</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>1696</v>
+        <v>1715</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>1699</v>
+        <v>1716</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>1696</v>
+        <v>1699</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>382</v>
+        <v>10</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>1696</v>
+        <v>1699</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>44</v>
+        <v>382</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>680</v>
+        <v>1699</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>10</v>
+        <v>1689</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>680</v>
+        <v>1695</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>700</v>
+        <v>1696</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>1039</v>
+        <v>1695</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>8</v>
+        <v>526</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>1039</v>
+        <v>1695</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>12</v>
+        <v>1697</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>1039</v>
+        <v>1695</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>146</v>
+        <v>1698</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>1039</v>
+        <v>1695</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>16</v>
+        <v>382</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>1039</v>
+        <v>1695</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>1039</v>
+        <v>680</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>1039</v>
+        <v>680</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>673</v>
+        <v>700</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>1039</v>
+        <v>1695</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>859</v>
+        <v>395</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>1039</v>
+        <v>1695</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>40</v>
+        <v>397</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>1039</v>
+        <v>1695</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>44</v>
+        <v>399</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>1039</v>
+        <v>1695</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1045</v>
+        <v>401</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>1039</v>
+        <v>1695</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>10</v>
+        <v>403</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>1039</v>
+        <v>1695</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>1047</v>
+        <v>405</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>1039</v>
+        <v>1695</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>42</v>
+        <v>407</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>1039</v>
+        <v>1695</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>38</v>
+        <v>409</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>1039</v>
+        <v>1695</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1070</v>
+        <v>411</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>1701</v>
+        <v>1695</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1690</v>
+        <v>322</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>1701</v>
+        <v>1737</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>1702</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>1712</v>
+      </c>
+      <c r="C47" s="3"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>1701</v>
+        <v>1737</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>1703</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>1713</v>
+      </c>
+      <c r="C48" s="3"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>1701</v>
+        <v>1737</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1704</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>1714</v>
+      </c>
+      <c r="C49" s="3"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>1701</v>
+        <v>1725</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>1705</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>1726</v>
+      </c>
+      <c r="C50" s="3"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>1701</v>
+        <v>1725</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>1706</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>1727</v>
+      </c>
+      <c r="C51" s="3"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>1701</v>
+        <v>1725</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>1707</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>1728</v>
+      </c>
+      <c r="C52" s="3"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>1701</v>
+        <v>1725</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>1708</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>1729</v>
+      </c>
+      <c r="C53" s="3"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>1701</v>
+        <v>1717</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>1709</v>
+        <v>60</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>1701</v>
+        <v>1717</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1710</v>
+        <v>40</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>1701</v>
+        <v>1717</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>1711</v>
+        <v>30</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>1234</v>
+        <v>1717</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>646</v>
+        <v>36</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>1693</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>1234</v>
+        <v>1717</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>648</v>
+        <v>12</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>1693</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>1234</v>
+        <v>1717</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>1693</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>1234</v>
+        <v>1718</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>1265</v>
+        <v>8</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>1693</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>1234</v>
+        <v>1718</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>1693</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>1314</v>
+        <v>1718</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>8</v>
+        <v>380</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
-        <v>1314</v>
+      <c r="A63" s="7" t="s">
+        <v>1718</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C63" s="3"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="7" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C64" s="3"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="7" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C65" s="3"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="7" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C66" s="3"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="7" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="7" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C68" s="3"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="7" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C69" s="3"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="7" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="C70" s="3"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="7" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C71" s="3"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="7" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="C72" s="3"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="7" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="C73" s="3"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="7" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C74" s="3"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="7" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C75" s="3"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="7" t="s">
+        <v>1718</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="3" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>1315</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>1317</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="3" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>1326</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="3" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>853</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="3" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="3" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="3" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="3" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="3" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>1695</v>
-      </c>
+      <c r="C76" s="3"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>1339</v>
+        <v>1719</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="3" t="s">
-        <v>1339</v>
+      <c r="A78" s="7" t="s">
+        <v>1719</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>395</v>
+      </c>
+      <c r="C78" s="3"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="3" t="s">
-        <v>1339</v>
+      <c r="A79" s="7" t="s">
+        <v>1719</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>859</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>397</v>
+      </c>
+      <c r="C79" s="3"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="3" t="s">
-        <v>1339</v>
+      <c r="A80" s="7" t="s">
+        <v>1719</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>1042</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>399</v>
+      </c>
+      <c r="C80" s="3"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="3" t="s">
-        <v>1339</v>
+      <c r="A81" s="7" t="s">
+        <v>1719</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>401</v>
+      </c>
+      <c r="C81" s="3"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
-        <v>1339</v>
+      <c r="A82" s="7" t="s">
+        <v>1719</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>403</v>
+      </c>
+      <c r="C82" s="3"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" s="3" t="s">
-        <v>1339</v>
+      <c r="A83" s="7" t="s">
+        <v>1719</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>405</v>
+      </c>
+      <c r="C83" s="3"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" s="3" t="s">
-        <v>1339</v>
+      <c r="A84" s="7" t="s">
+        <v>1719</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>407</v>
+      </c>
+      <c r="C84" s="3"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="3" t="s">
-        <v>1339</v>
+      <c r="A85" s="7" t="s">
+        <v>1719</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>409</v>
+      </c>
+      <c r="C85" s="3"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="3" t="s">
-        <v>1339</v>
+      <c r="A86" s="7" t="s">
+        <v>1719</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>862</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>411</v>
+      </c>
+      <c r="C86" s="3"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" s="3" t="s">
-        <v>1339</v>
+      <c r="A87" s="7" t="s">
+        <v>1719</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>864</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>322</v>
+      </c>
+      <c r="C87" s="3"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" s="3" t="s">
-        <v>1339</v>
+      <c r="A88" s="7" t="s">
+        <v>1719</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>1348</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>383</v>
+      </c>
+      <c r="C88" s="3"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" s="3" t="s">
-        <v>1373</v>
+      <c r="A89" s="7" t="s">
+        <v>1719</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C89" s="3"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" s="3" t="s">
-        <v>1373</v>
+      <c r="A90" s="7" t="s">
+        <v>1719</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>1742</v>
+      </c>
+      <c r="C90" s="3"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" s="3" t="s">
-        <v>1373</v>
+      <c r="A91" s="7" t="s">
+        <v>1719</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>383</v>
+      </c>
+      <c r="C91" s="3"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" s="3" t="s">
-        <v>1373</v>
+      <c r="A92" s="7" t="s">
+        <v>1719</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>387</v>
+      </c>
+      <c r="C92" s="3"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" s="3" t="s">
-        <v>1653</v>
+      <c r="A93" s="7" t="s">
+        <v>1719</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>553</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>1695</v>
-      </c>
+        <v>1743</v>
+      </c>
+      <c r="C93" s="3"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
-        <v>1653</v>
+        <v>1721</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>1688</v>
+        <v>1091</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>1695</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
-        <v>1653</v>
+        <v>1721</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>1689</v>
+        <v>1093</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>1695</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
-        <v>1653</v>
+        <v>1721</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>1690</v>
+        <v>1106</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>1695</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
-        <v>1653</v>
+        <v>1723</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>1691</v>
+        <v>1269</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>1695</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>1653</v>
+        <v>1723</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>1692</v>
+        <v>650</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>1695</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
-        <v>1653</v>
+        <v>1723</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>1695</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>1653</v>
+        <v>1720</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>526</v>
+        <v>1091</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>1653</v>
+        <v>1720</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>530</v>
+        <v>1093</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>1653</v>
+        <v>1720</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>532</v>
+        <v>1106</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
-        <v>1653</v>
+        <v>1039</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>534</v>
+        <v>8</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
-        <v>1653</v>
+        <v>1039</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>382</v>
+        <v>12</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>1653</v>
+        <v>1039</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>544</v>
+        <v>146</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
-        <v>1653</v>
+        <v>1039</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>547</v>
+        <v>16</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>1653</v>
+        <v>1039</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
-        <v>1653</v>
+        <v>1039</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>26</v>
+        <v>673</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>1653</v>
+        <v>1039</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>4</v>
+        <v>859</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
-        <v>1712</v>
+        <v>1039</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>1688</v>
+        <v>40</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
-        <v>1712</v>
+        <v>1039</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>1689</v>
+        <v>44</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
-        <v>1712</v>
+        <v>1039</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>1713</v>
+        <v>1045</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
-        <v>1712</v>
+        <v>1039</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>1714</v>
+        <v>10</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
-        <v>1712</v>
+        <v>1039</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>1715</v>
+        <v>1047</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
-        <v>1716</v>
+        <v>1039</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
-        <v>1716</v>
+        <v>1039</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>1690</v>
+        <v>38</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
-        <v>1716</v>
+        <v>1039</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>1717</v>
+        <v>1070</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
-        <v>1718</v>
+        <v>1711</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>60</v>
+        <v>1687</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
-        <v>1718</v>
+        <v>1711</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>40</v>
+        <v>1688</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
-        <v>1718</v>
+        <v>1711</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>30</v>
+        <v>1712</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>1718</v>
+        <v>1711</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>36</v>
+        <v>1713</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
-        <v>1718</v>
+        <v>1711</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>12</v>
+        <v>1714</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>1718</v>
+        <v>1700</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>44</v>
+        <v>1689</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
-        <v>1719</v>
+        <v>1700</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>8</v>
+        <v>1701</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>1719</v>
+        <v>1700</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>20</v>
+        <v>1702</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
-        <v>1719</v>
+        <v>1700</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>380</v>
+        <v>1703</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
-        <v>1720</v>
+        <v>1700</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>24</v>
+        <v>1704</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
-        <v>1721</v>
+        <v>1700</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>1091</v>
+        <v>1705</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
-        <v>1721</v>
+        <v>1700</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>1093</v>
+        <v>1706</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
-        <v>1721</v>
+        <v>1700</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>1106</v>
+        <v>1707</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
-        <v>1722</v>
+        <v>1700</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>1091</v>
+        <v>1708</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>1723</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
-        <v>1722</v>
+        <v>1700</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>1093</v>
+        <v>1709</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>1723</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
-        <v>1722</v>
+        <v>1700</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>1106</v>
+        <v>1710</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>1723</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
-        <v>1724</v>
+        <v>1234</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>1269</v>
+        <v>646</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>1725</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A135" s="3" t="s">
-        <v>1724</v>
+      <c r="A135" s="8" t="s">
+        <v>1234</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>1725</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A136" s="3" t="s">
-        <v>1724</v>
+      <c r="A136" s="8" t="s">
+        <v>1234</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>1725</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A137" s="6" t="s">
-        <v>1719</v>
+      <c r="A137" s="8" t="s">
+        <v>1234</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="C137" s="3"/>
+        <v>1265</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>1692</v>
+      </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A138" s="6" t="s">
-        <v>1719</v>
+      <c r="A138" s="8" t="s">
+        <v>1234</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="C138" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>1692</v>
+      </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A139" s="6" t="s">
-        <v>1719</v>
+      <c r="A139" s="8" t="s">
+        <v>1314</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="C139" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A140" s="6" t="s">
-        <v>1719</v>
+      <c r="A140" s="8" t="s">
+        <v>1314</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="C140" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A141" s="6" t="s">
-        <v>1719</v>
+      <c r="A141" s="8" t="s">
+        <v>1314</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="C141" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A142" s="6" t="s">
-        <v>1719</v>
+      <c r="A142" s="8" t="s">
+        <v>1314</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="C142" s="3"/>
+        <v>382</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143" s="6" t="s">
-        <v>1719</v>
+      <c r="A143" s="8" t="s">
+        <v>1314</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="C143" s="3"/>
+        <v>1315</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A144" s="6" t="s">
-        <v>1719</v>
+      <c r="A144" s="8" t="s">
+        <v>1314</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="C144" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" s="6" t="s">
-        <v>1719</v>
+      <c r="A145" s="8" t="s">
+        <v>1314</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="C145" s="3"/>
+        <v>1317</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" s="6" t="s">
-        <v>1719</v>
+      <c r="A146" s="8" t="s">
+        <v>1314</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="C146" s="3"/>
+        <v>1326</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" s="6" t="s">
-        <v>1719</v>
+      <c r="A147" s="8" t="s">
+        <v>1314</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="C147" s="3"/>
+        <v>853</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" s="6" t="s">
-        <v>1719</v>
+      <c r="A148" s="8" t="s">
+        <v>1740</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>322</v>
+        <v>1712</v>
       </c>
       <c r="C148" s="3"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149" s="6" t="s">
-        <v>1719</v>
+      <c r="A149" s="8" t="s">
+        <v>1740</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>383</v>
+        <v>1713</v>
       </c>
       <c r="C149" s="3"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A150" s="6" t="s">
-        <v>1719</v>
+      <c r="A150" s="8" t="s">
+        <v>1740</v>
       </c>
       <c r="B150" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C150" s="3"/>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A151" s="8" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C151" s="3"/>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A152" s="8" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C152" s="3"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A153" s="8" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C153" s="3"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A154" s="8" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C154" s="3"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A155" s="8" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C155" s="3"/>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A156" s="8" t="s">
+        <v>1739</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C156" s="3"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A157" s="8" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A158" s="8" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A159" s="8" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A160" s="8" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A161" s="8" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B161" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C150" s="3"/>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A151" s="6" t="s">
-        <v>1720</v>
-      </c>
-      <c r="B151" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="C151" s="3"/>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A152" s="6" t="s">
-        <v>1720</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="C152" s="3"/>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A153" s="6" t="s">
-        <v>1720</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="C153" s="3"/>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A154" s="6" t="s">
-        <v>1720</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="C154" s="3"/>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A155" s="6" t="s">
-        <v>1720</v>
-      </c>
-      <c r="B155" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="C155" s="3"/>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A156" s="6" t="s">
-        <v>1720</v>
-      </c>
-      <c r="B156" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="C156" s="3"/>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A157" s="6" t="s">
-        <v>1720</v>
-      </c>
-      <c r="B157" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="C157" s="3"/>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A158" s="6" t="s">
-        <v>1720</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="C158" s="3"/>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A159" s="6" t="s">
-        <v>1720</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="C159" s="3"/>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A160" s="6" t="s">
-        <v>1720</v>
-      </c>
-      <c r="B160" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="C160" s="3"/>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A161" s="6" t="s">
-        <v>1720</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="C161" s="3"/>
+      <c r="C161" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A162" s="6" t="s">
-        <v>1720</v>
+      <c r="A162" s="8" t="s">
+        <v>1339</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C162" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A163" s="6" t="s">
-        <v>1720</v>
+      <c r="A163" s="8" t="s">
+        <v>1339</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>1743</v>
-      </c>
-      <c r="C163" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A164" s="6" t="s">
-        <v>1720</v>
+      <c r="A164" s="8" t="s">
+        <v>1339</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="C164" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A165" s="6" t="s">
-        <v>1720</v>
+      <c r="A165" s="3" t="s">
+        <v>1339</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="C165" s="3"/>
+        <v>859</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A166" s="6" t="s">
-        <v>1720</v>
+      <c r="A166" s="3" t="s">
+        <v>1339</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1744</v>
-      </c>
-      <c r="C166" s="3"/>
+        <v>1042</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="3" t="s">
-        <v>1653</v>
+        <v>1339</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>1745</v>
-      </c>
-      <c r="C167" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="3" t="s">
-        <v>1696</v>
+        <v>1339</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="C168" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="3" t="s">
-        <v>1696</v>
+        <v>1339</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="C169" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="3" t="s">
-        <v>1696</v>
+        <v>1339</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="C170" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="3" t="s">
-        <v>1696</v>
+        <v>1339</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="C171" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="3" t="s">
-        <v>1696</v>
+        <v>1339</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="C172" s="3"/>
+        <v>862</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="3" t="s">
-        <v>1696</v>
+        <v>1339</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="C173" s="3"/>
+        <v>864</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="3" t="s">
-        <v>1696</v>
+        <v>1339</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="C174" s="3"/>
+        <v>1348</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="3" t="s">
-        <v>1696</v>
+        <v>1373</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="C175" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="3" t="s">
-        <v>1696</v>
+        <v>1373</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="C176" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="3" t="s">
-        <v>1696</v>
+        <v>1373</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="C177" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="3" t="s">
-        <v>1735</v>
+        <v>1373</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>1715</v>
-      </c>
-      <c r="C178" s="3"/>
+        <v>538</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="3" t="s">
-        <v>1735</v>
+        <v>1741</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="C179" s="3"/>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" s="3" t="s">
-        <v>1735</v>
+        <v>1741</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>1736</v>
+        <v>1713</v>
       </c>
       <c r="C180" s="3"/>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="3" t="s">
-        <v>1737</v>
+        <v>1741</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>1713</v>
+        <v>1714</v>
       </c>
       <c r="C181" s="3"/>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="3" t="s">
-        <v>1737</v>
+        <v>1653</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C182" s="3"/>
+        <v>553</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" s="3" t="s">
-        <v>1737</v>
+        <v>1653</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>1715</v>
-      </c>
-      <c r="C183" s="3"/>
+        <v>1687</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="3" t="s">
-        <v>1738</v>
+        <v>1653</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>1713</v>
-      </c>
-      <c r="C184" s="3"/>
+        <v>1688</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" s="3" t="s">
-        <v>1738</v>
+        <v>1653</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C185" s="3"/>
+        <v>1689</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" s="3" t="s">
-        <v>1738</v>
+        <v>1653</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>1715</v>
-      </c>
-      <c r="C186" s="3"/>
+        <v>1690</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" s="3" t="s">
-        <v>1739</v>
+        <v>1653</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>1713</v>
-      </c>
-      <c r="C187" s="3"/>
+        <v>1691</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" s="3" t="s">
-        <v>1739</v>
+        <v>1653</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C188" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" s="3" t="s">
-        <v>1739</v>
+        <v>1653</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>1715</v>
-      </c>
-      <c r="C189" s="3"/>
+        <v>526</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" s="3" t="s">
-        <v>1740</v>
+        <v>1653</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>1713</v>
-      </c>
-      <c r="C190" s="3"/>
+        <v>530</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" s="3" t="s">
-        <v>1739</v>
+        <v>1653</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C191" s="3"/>
+        <v>532</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" s="3" t="s">
-        <v>1739</v>
+        <v>1653</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>1715</v>
-      </c>
-      <c r="C192" s="3"/>
+        <v>534</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" s="3" t="s">
-        <v>1741</v>
+        <v>1653</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>1713</v>
-      </c>
-      <c r="C193" s="3"/>
+        <v>382</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="3" t="s">
-        <v>1741</v>
+        <v>1653</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C194" s="3"/>
+        <v>544</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" s="3" t="s">
-        <v>1741</v>
+        <v>1653</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>1715</v>
-      </c>
-      <c r="C195" s="3"/>
+        <v>547</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="3" t="s">
-        <v>1742</v>
+        <v>1653</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>1713</v>
-      </c>
-      <c r="C196" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" s="3" t="s">
-        <v>1742</v>
+        <v>1653</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C197" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" s="3" t="s">
-        <v>1742</v>
+        <v>1653</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>1715</v>
-      </c>
-      <c r="C198" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>1694</v>
+      </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" s="3" t="s">
-        <v>1726</v>
+        <v>1653</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>1727</v>
+        <v>1744</v>
       </c>
       <c r="C199" s="3"/>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" s="3" t="s">
-        <v>1726</v>
+        <v>1734</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>1728</v>
+        <v>1714</v>
       </c>
       <c r="C200" s="3"/>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" s="3" t="s">
-        <v>1726</v>
+        <v>1734</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>1729</v>
+        <v>1712</v>
       </c>
       <c r="C201" s="3"/>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" s="3" t="s">
-        <v>1726</v>
+        <v>1734</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>1730</v>
+        <v>1735</v>
       </c>
       <c r="C202" s="3"/>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A203" s="3" t="s">
-        <v>1731</v>
-      </c>
-      <c r="B203" s="3" t="s">
-        <v>1732</v>
-      </c>
-      <c r="C203" s="3"/>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A204" s="3" t="s">
-        <v>1731</v>
-      </c>
-      <c r="B204" s="3" t="s">
-        <v>1733</v>
-      </c>
-      <c r="C204" s="3"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B101:B104">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="B100:B103">
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B106:B109">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="B105:B107">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -41407,7 +41479,7 @@
           <x14:formula1>
             <xm:f>'C:\Users\09118\Desktop\[Baseline Spreadsheet AL_Fields.xlsx]Tables'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A87 A97:A98 A168:A177</xm:sqref>
+          <xm:sqref>A96:A97 A166:A175 A2:A86</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -41431,7 +41503,7 @@
   <sheetData>
     <row r="6" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: Added new feature classes.
</commit_message>
<xml_diff>
--- a/AL_Fields_Revised.xlsx
+++ b/AL_Fields_Revised.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\gisappser2\Engineering_GIS\Domiano_Robert\USIC\PythonScripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B050D2-22F9-4FD3-9F3B-060642B9CFBB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E99C6A-0902-4C63-8966-BAC2C9284AD7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{367E046B-1E4C-49F6-BAFA-71796CED2EB1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1 (2)" sheetId="6" r:id="rId1"/>
-    <sheet name="RecordedFields" sheetId="4" r:id="rId2"/>
-    <sheet name="FieldsToAdd" sheetId="5" r:id="rId3"/>
+    <sheet name="RecordedFields" sheetId="4" r:id="rId1"/>
+    <sheet name="FieldsToAdd" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet1 (2)" sheetId="6" r:id="rId3"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet1 (2)'!$A$1:$A$2960</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sheet1 (2)'!$A$1:$A$2960</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9450" uniqueCount="1751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9464" uniqueCount="1760">
   <si>
     <t>Table</t>
   </si>
@@ -5186,27 +5186,9 @@
     <t>labeltext</t>
   </si>
   <si>
-    <t>GISADMIN.AbandonedService</t>
-  </si>
-  <si>
-    <t>GISADMIN.CPANODE</t>
-  </si>
-  <si>
-    <t>GISADMIN.CPTestPoint</t>
-  </si>
-  <si>
-    <t>GISADMIN.ServiceText</t>
-  </si>
-  <si>
-    <t>gisadmin.miscellaneousText</t>
-  </si>
-  <si>
     <t>gisadmin.landbase</t>
   </si>
   <si>
-    <t>gisadmin.projectBoundary</t>
-  </si>
-  <si>
     <t>gisadmin.projectdata</t>
   </si>
   <si>
@@ -5270,9 +5252,6 @@
     <t>LOCATIONDIRECTION</t>
   </si>
   <si>
-    <t>Is URL wanted for Customer shp?</t>
-  </si>
-  <si>
     <t>Do not need. Script this out.</t>
   </si>
   <si>
@@ -5286,6 +5265,54 @@
   </si>
   <si>
     <t>Not necessary - use Material Code instead</t>
+  </si>
+  <si>
+    <t>CPTest Point</t>
+  </si>
+  <si>
+    <t>Misc Text</t>
+  </si>
+  <si>
+    <t>project boundary</t>
+  </si>
+  <si>
+    <t>service text</t>
+  </si>
+  <si>
+    <t>cp anode</t>
+  </si>
+  <si>
+    <t>abandon Service</t>
+  </si>
+  <si>
+    <t>Gas lamp</t>
+  </si>
+  <si>
+    <t>street number</t>
+  </si>
+  <si>
+    <t>street name</t>
+  </si>
+  <si>
+    <t>street suffix</t>
+  </si>
+  <si>
+    <t>main authorization number text</t>
+  </si>
+  <si>
+    <t>Location description text</t>
+  </si>
+  <si>
+    <t>detail annotation text</t>
+  </si>
+  <si>
+    <t>station plus text</t>
+  </si>
+  <si>
+    <t>notes text</t>
+  </si>
+  <si>
+    <t>Leader lines</t>
   </si>
 </sst>
 </file>
@@ -5369,7 +5396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -5379,49 +5406,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5470,6 +5464,26 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5538,15 +5552,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1294518F-F526-4B7B-9FA0-AAD867AF8FD9}" name="Table1" displayName="Table1" ref="A1:C202" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:C202" xr:uid="{F75189C3-0D66-4B7E-B1E3-9B62E992FBAD}"/>
-  <sortState ref="A2:C202">
-    <sortCondition ref="A1:A202"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1294518F-F526-4B7B-9FA0-AAD867AF8FD9}" name="Table1" displayName="Table1" ref="A1:C212" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:C212" xr:uid="{F75189C3-0D66-4B7E-B1E3-9B62E992FBAD}"/>
+  <sortState ref="A2:C200">
+    <sortCondition ref="A1:A200"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{B45FB957-20AF-4788-ACCE-9607C2A5885E}" name="fromTable" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{DAC79196-D75B-4C5A-BA0D-ACA19E0274C7}" name="keepList" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{A155A2E6-B443-4176-BE9B-DD01B1938F64}" name="Datalayer" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{B45FB957-20AF-4788-ACCE-9607C2A5885E}" name="fromTable" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{DAC79196-D75B-4C5A-BA0D-ACA19E0274C7}" name="keepList" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{A155A2E6-B443-4176-BE9B-DD01B1938F64}" name="Datalayer" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5848,12 +5862,2269 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1E5225-34EE-4EC7-BF9B-DBF232E3BF15}">
+  <dimension ref="A1:C212"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="A216" sqref="A216"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1685</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1693</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>1730</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>1730</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>1730</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>1726</v>
+      </c>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>1724</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>1716</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>1696</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>1698</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>1697</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="9" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>1722</v>
+      </c>
+      <c r="C50" s="3"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>1721</v>
+      </c>
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>1723</v>
+      </c>
+      <c r="C52" s="3"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>1720</v>
+      </c>
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C60" s="3"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C61" s="3"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="C62" s="3"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C63" s="3"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C64" s="3"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C65" s="3"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="C66" s="3"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C68" s="3"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C69" s="3"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="C70" s="3"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C71" s="3"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C73" s="3"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C74" s="3"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C75" s="3"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C77" s="3"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C78" s="3"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C79" s="3"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="C80" s="3"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C82" s="3"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C83" s="3"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C84" s="3"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="C85" s="3"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C86" s="3"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C87" s="3"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C88" s="3"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="C89" s="3"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90" s="3"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>1736</v>
+      </c>
+      <c r="C91" s="3"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C92" s="3"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C93" s="3"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="3" t="s">
+        <v>1745</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>1717</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="3" t="s">
+        <v>1745</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>1717</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="3" t="s">
+        <v>1745</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>1717</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="3" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="3" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="3" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="3" t="s">
+        <v>1747</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="3" t="s">
+        <v>1747</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="3" t="s">
+        <v>1747</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="3" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="3" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" s="3" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" s="3" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="3" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="3" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" s="3" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="3" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="9" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="9" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="9" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="9" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="9" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>859</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="9" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="3" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="3" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="3" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="9" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>1687</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="3" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>1688</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="3" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="3" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>1704</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="3" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="3" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>1702</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="3" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="3" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="3" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>1706</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="3" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="3" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="3" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>1708</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" s="3" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" s="3" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>1710</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" s="3" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" s="8" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" s="8" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" s="8" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" s="8" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" s="8" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" s="8" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" s="8" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" s="8" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" s="8" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" s="8" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>1317</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A145" s="8" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146" s="8" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147" s="8" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148" s="8" t="s">
+        <v>1734</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C148" s="3"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A149" s="8" t="s">
+        <v>1734</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C149" s="3"/>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A150" s="8" t="s">
+        <v>1734</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C150" s="3"/>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A151" s="8" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C151" s="3"/>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A152" s="8" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C152" s="3"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A153" s="8" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C153" s="3"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A154" s="8" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C154" s="3"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A155" s="8" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C155" s="3"/>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A156" s="8" t="s">
+        <v>1733</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C156" s="3"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A157" s="8" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A158" s="8" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A159" s="8" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A160" s="8" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A161" s="8" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162" s="8" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A163" s="8" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A164" s="8" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>864</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A165" s="3" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A166" s="9" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A167" s="9" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A168" s="9" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A169" s="9" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A170" s="9" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>859</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A171" s="9" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A172" s="9" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A173" s="3" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174" s="3" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>862</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A175" s="3" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A176" s="3" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A177" s="3" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A178" s="9" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A179" s="3" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C179" s="3"/>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A180" s="3" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C180" s="3"/>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A181" s="3" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C181" s="3"/>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A182" s="3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>1690</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A183" s="3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A184" s="3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A185" s="3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A186" s="3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A187" s="3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A188" s="3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A189" s="3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>1738</v>
+      </c>
+      <c r="C189" s="3"/>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A190" s="3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A191" s="9" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A192" s="3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A193" s="3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A194" s="3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A195" s="3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A196" s="3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A197" s="3" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A198" s="3" t="s">
+        <v>1728</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C198" s="3"/>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A199" s="9" t="s">
+        <v>1728</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>1729</v>
+      </c>
+      <c r="C199" s="3"/>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A200" s="3" t="s">
+        <v>1728</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C200" s="3"/>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A201" s="3" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>1720</v>
+      </c>
+      <c r="C201" s="3"/>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A202" s="3" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="C202" s="3"/>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A203" s="3" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>1752</v>
+      </c>
+      <c r="C203" s="3"/>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A204" s="3" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>1753</v>
+      </c>
+      <c r="C204" s="3"/>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A205" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C205" s="3"/>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A206" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C206" s="3"/>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A207" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C207" s="3"/>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A208" s="3" t="s">
+        <v>1755</v>
+      </c>
+      <c r="B208" s="3"/>
+      <c r="C208" s="3"/>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A209" s="3" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B209" s="3"/>
+      <c r="C209" s="3"/>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A210" s="3" t="s">
+        <v>1757</v>
+      </c>
+      <c r="B210" s="3"/>
+      <c r="C210" s="3"/>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A211" s="3" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B211" s="3"/>
+      <c r="C211" s="3"/>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A212" s="3" t="s">
+        <v>1759</v>
+      </c>
+      <c r="B212" s="3"/>
+      <c r="C212" s="3"/>
+    </row>
+  </sheetData>
+  <sortState ref="F181:F182">
+    <sortCondition ref="F182"/>
+  </sortState>
+  <conditionalFormatting sqref="B100:B103">
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B105:B107">
+    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{AA5AD403-DFDE-45B5-9FB9-303BAC8E6091}">
+          <x14:formula1>
+            <xm:f>'C:\Users\09118\Desktop\[Baseline Spreadsheet AL_Fields.xlsx]Tables'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>A97:A99 A166:A175 A2:A93</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6F9BE1-CA72-4A1E-B3E5-1D5DC86488E4}">
+  <dimension ref="C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>1727</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426C2F6F-D76E-4751-9350-DDCF1863B36A}">
   <dimension ref="A1:W2960"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5904,7 +8175,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>1746</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
@@ -6347,7 +8618,7 @@
         <v>11</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>1747</v>
+        <v>1740</v>
       </c>
       <c r="E18" s="3"/>
       <c r="G18" s="3"/>
@@ -6379,7 +8650,7 @@
         <v>44</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>1747</v>
+        <v>1740</v>
       </c>
       <c r="E19" s="3"/>
       <c r="G19" s="3"/>
@@ -6411,7 +8682,7 @@
         <v>11</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>1747</v>
+        <v>1740</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -6444,7 +8715,7 @@
         <v>44</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>1747</v>
+        <v>1740</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -6694,7 +8965,7 @@
         <v>700</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>1748</v>
+        <v>1741</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -6727,7 +8998,7 @@
         <v>159</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>1749</v>
+        <v>1742</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -6824,7 +9095,7 @@
         <v>21</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>1750</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -39296,7 +41567,7 @@
   </sheetData>
   <autoFilter ref="A1:A2960" xr:uid="{23E46DE6-C876-4310-B0A6-27F6C702C110}">
     <sortState ref="A2:C2960">
-      <sortCondition sortBy="cellColor" ref="A1:A2960" dxfId="5"/>
+      <sortCondition sortBy="cellColor" ref="A1:A2960" dxfId="1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -39331,2182 +41602,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1E5225-34EE-4EC7-BF9B-DBF232E3BF15}">
-  <dimension ref="A1:G202"/>
-  <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B170" sqref="B170"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.88671875" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>1686</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1685</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1693</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1694</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1745</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>1736</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>1712</v>
-      </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>1736</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>1713</v>
-      </c>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>1736</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>1730</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>1731</v>
-      </c>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>1730</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>1732</v>
-      </c>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>1715</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>1715</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>1689</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>1715</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>1716</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>1699</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>1699</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>1699</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>1689</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>1696</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>1697</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>1698</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>700</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>1695</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
-        <v>1737</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>1712</v>
-      </c>
-      <c r="C47" s="3"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
-        <v>1737</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>1713</v>
-      </c>
-      <c r="C48" s="3"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
-        <v>1737</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C49" s="3"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>1725</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>1726</v>
-      </c>
-      <c r="C50" s="3"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
-        <v>1725</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>1727</v>
-      </c>
-      <c r="C51" s="3"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="3" t="s">
-        <v>1725</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>1728</v>
-      </c>
-      <c r="C52" s="3"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="3" t="s">
-        <v>1725</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>1729</v>
-      </c>
-      <c r="C53" s="3"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
-        <v>1717</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="3" t="s">
-        <v>1717</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="3" t="s">
-        <v>1717</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
-        <v>1717</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
-        <v>1717</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="3" t="s">
-        <v>1717</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="3" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="7" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="C63" s="3"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="7" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="C64" s="3"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="7" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="C65" s="3"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="7" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="C66" s="3"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="7" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="C67" s="3"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="7" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="C68" s="3"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="7" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="C69" s="3"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="7" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="C70" s="3"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="7" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="C71" s="3"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="7" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="C72" s="3"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="7" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="C73" s="3"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="7" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="C74" s="3"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="7" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="C75" s="3"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="7" t="s">
-        <v>1718</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C76" s="3"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="3" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="7" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="C78" s="3"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="7" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="C79" s="3"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="7" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="C80" s="3"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="7" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="C81" s="3"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="7" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="C82" s="3"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" s="7" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="C83" s="3"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" s="7" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="C84" s="3"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="7" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="C85" s="3"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="7" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="C86" s="3"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" s="7" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="C87" s="3"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" s="7" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="C88" s="3"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" s="7" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C89" s="3"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" s="7" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>1742</v>
-      </c>
-      <c r="C90" s="3"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" s="7" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="C91" s="3"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" s="7" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="C92" s="3"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" s="7" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>1743</v>
-      </c>
-      <c r="C93" s="3"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" s="3" t="s">
-        <v>1721</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>1091</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>1722</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" s="3" t="s">
-        <v>1721</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>1093</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>1722</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="3" t="s">
-        <v>1721</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>1106</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>1722</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="3" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>1269</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>1724</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="3" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>650</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>1724</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="3" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>1724</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="3" t="s">
-        <v>1720</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>1091</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="3" t="s">
-        <v>1720</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>1093</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="3" t="s">
-        <v>1720</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>1106</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" s="3" t="s">
-        <v>1039</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="3" t="s">
-        <v>1039</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" s="3" t="s">
-        <v>1039</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" s="3" t="s">
-        <v>1039</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" s="3" t="s">
-        <v>1039</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" s="3" t="s">
-        <v>1039</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>673</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" s="3" t="s">
-        <v>1039</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>859</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" s="3" t="s">
-        <v>1039</v>
-      </c>
-      <c r="B110" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" s="3" t="s">
-        <v>1039</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" s="3" t="s">
-        <v>1039</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>1045</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" s="3" t="s">
-        <v>1039</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" s="3" t="s">
-        <v>1039</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>1047</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" s="3" t="s">
-        <v>1039</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" s="3" t="s">
-        <v>1039</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A117" s="3" t="s">
-        <v>1039</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>1070</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118" s="3" t="s">
-        <v>1711</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>1687</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" s="3" t="s">
-        <v>1711</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>1688</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120" s="3" t="s">
-        <v>1711</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>1712</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121" s="3" t="s">
-        <v>1711</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>1713</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122" s="3" t="s">
-        <v>1711</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123" s="3" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>1689</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A124" s="3" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>1701</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125" s="3" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>1702</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126" s="3" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>1703</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A127" s="3" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>1704</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A128" s="3" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>1705</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129" s="3" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>1706</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A130" s="3" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>1707</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A131" s="3" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>1708</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A132" s="3" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>1709</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A133" s="3" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>1710</v>
-      </c>
-      <c r="C133" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A134" s="3" t="s">
-        <v>1234</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>646</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>1692</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A135" s="8" t="s">
-        <v>1234</v>
-      </c>
-      <c r="B135" s="3" t="s">
-        <v>648</v>
-      </c>
-      <c r="C135" s="3" t="s">
-        <v>1692</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A136" s="8" t="s">
-        <v>1234</v>
-      </c>
-      <c r="B136" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C136" s="3" t="s">
-        <v>1692</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A137" s="8" t="s">
-        <v>1234</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>1265</v>
-      </c>
-      <c r="C137" s="3" t="s">
-        <v>1692</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A138" s="8" t="s">
-        <v>1234</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C138" s="3" t="s">
-        <v>1692</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A139" s="8" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C139" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A140" s="8" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A141" s="8" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B141" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C141" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A142" s="8" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="C142" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143" s="8" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>1315</v>
-      </c>
-      <c r="C143" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A144" s="8" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B144" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C144" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" s="8" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>1317</v>
-      </c>
-      <c r="C145" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" s="8" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B146" s="3" t="s">
-        <v>1326</v>
-      </c>
-      <c r="C146" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" s="8" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B147" s="3" t="s">
-        <v>853</v>
-      </c>
-      <c r="C147" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" s="8" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B148" s="3" t="s">
-        <v>1712</v>
-      </c>
-      <c r="C148" s="3"/>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149" s="8" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B149" s="3" t="s">
-        <v>1713</v>
-      </c>
-      <c r="C149" s="3"/>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A150" s="8" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B150" s="3" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C150" s="3"/>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A151" s="8" t="s">
-        <v>1738</v>
-      </c>
-      <c r="B151" s="3" t="s">
-        <v>1712</v>
-      </c>
-      <c r="C151" s="3"/>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A152" s="8" t="s">
-        <v>1738</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>1713</v>
-      </c>
-      <c r="C152" s="3"/>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A153" s="8" t="s">
-        <v>1738</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C153" s="3"/>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A154" s="8" t="s">
-        <v>1738</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>1713</v>
-      </c>
-      <c r="C154" s="3"/>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A155" s="8" t="s">
-        <v>1738</v>
-      </c>
-      <c r="B155" s="3" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C155" s="3"/>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A156" s="8" t="s">
-        <v>1739</v>
-      </c>
-      <c r="B156" s="3" t="s">
-        <v>1712</v>
-      </c>
-      <c r="C156" s="3"/>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A157" s="8" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B157" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C157" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A158" s="8" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C158" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A159" s="8" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A160" s="8" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B160" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C160" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A161" s="8" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A162" s="8" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A163" s="8" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C163" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A164" s="8" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C164" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A165" s="3" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B165" s="3" t="s">
-        <v>859</v>
-      </c>
-      <c r="C165" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A166" s="3" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B166" s="3" t="s">
-        <v>1042</v>
-      </c>
-      <c r="C166" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A167" s="3" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B167" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C167" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A168" s="3" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B168" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C168" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A169" s="3" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B169" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C169" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A170" s="3" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B170" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A171" s="3" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C171" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A172" s="3" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B172" s="3" t="s">
-        <v>862</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A173" s="3" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>864</v>
-      </c>
-      <c r="C173" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A174" s="3" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>1348</v>
-      </c>
-      <c r="C174" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A175" s="3" t="s">
-        <v>1373</v>
-      </c>
-      <c r="B175" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C175" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A176" s="3" t="s">
-        <v>1373</v>
-      </c>
-      <c r="B176" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C176" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A177" s="3" t="s">
-        <v>1373</v>
-      </c>
-      <c r="B177" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C177" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A178" s="3" t="s">
-        <v>1373</v>
-      </c>
-      <c r="B178" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="C178" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A179" s="3" t="s">
-        <v>1741</v>
-      </c>
-      <c r="B179" s="3" t="s">
-        <v>1712</v>
-      </c>
-      <c r="C179" s="3"/>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A180" s="3" t="s">
-        <v>1741</v>
-      </c>
-      <c r="B180" s="3" t="s">
-        <v>1713</v>
-      </c>
-      <c r="C180" s="3"/>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A181" s="3" t="s">
-        <v>1741</v>
-      </c>
-      <c r="B181" s="3" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C181" s="3"/>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A182" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="B182" s="3" t="s">
-        <v>553</v>
-      </c>
-      <c r="C182" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A183" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="B183" s="3" t="s">
-        <v>1687</v>
-      </c>
-      <c r="C183" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A184" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>1688</v>
-      </c>
-      <c r="C184" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A185" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="B185" s="3" t="s">
-        <v>1689</v>
-      </c>
-      <c r="C185" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A186" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="B186" s="3" t="s">
-        <v>1690</v>
-      </c>
-      <c r="C186" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A187" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="B187" s="3" t="s">
-        <v>1691</v>
-      </c>
-      <c r="C187" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A188" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="B188" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C188" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A189" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="B189" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="C189" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A190" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="B190" s="3" t="s">
-        <v>530</v>
-      </c>
-      <c r="C190" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A191" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="B191" s="3" t="s">
-        <v>532</v>
-      </c>
-      <c r="C191" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A192" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>534</v>
-      </c>
-      <c r="C192" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A193" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="B193" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="C193" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A194" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="B194" s="3" t="s">
-        <v>544</v>
-      </c>
-      <c r="C194" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A195" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>547</v>
-      </c>
-      <c r="C195" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A196" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="B196" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C196" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A197" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="B197" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C197" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A198" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="B198" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C198" s="3" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A199" s="3" t="s">
-        <v>1653</v>
-      </c>
-      <c r="B199" s="3" t="s">
-        <v>1744</v>
-      </c>
-      <c r="C199" s="3"/>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A200" s="3" t="s">
-        <v>1734</v>
-      </c>
-      <c r="B200" s="3" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C200" s="3"/>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A201" s="3" t="s">
-        <v>1734</v>
-      </c>
-      <c r="B201" s="3" t="s">
-        <v>1712</v>
-      </c>
-      <c r="C201" s="3"/>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A202" s="3" t="s">
-        <v>1734</v>
-      </c>
-      <c r="B202" s="3" t="s">
-        <v>1735</v>
-      </c>
-      <c r="C202" s="3"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B100:B103">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B105:B107">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{AA5AD403-DFDE-45B5-9FB9-303BAC8E6091}">
-          <x14:formula1>
-            <xm:f>'C:\Users\09118\Desktop\[Baseline Spreadsheet AL_Fields.xlsx]Tables'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>A96:A97 A166:A175 A2:A86</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6F9BE1-CA72-4A1E-B3E5-1D5DC86488E4}">
-  <dimension ref="C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="A1:B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>1733</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>